<commit_message>
(2024.02.20) 1) Separate a file as MVC pattern 2) Set a command file import UI 3) Import a command file from a user-specified directory 4) Change a main window title 5) apply a command version display
</commit_message>
<xml_diff>
--- a/Command/Command.xlsx
+++ b/Command/Command.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chalie/Desktop/Python/SL-640C/Command/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D8294F-5C7F-334D-B0BB-4D29471AD24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1912635B-395A-4440-A34B-6CB40E13A5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{79FED000-970D-0E48-B65E-FB5160DD82FF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="433">
   <si>
     <r>
       <rPr>
@@ -4044,10 +4044,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Rev.2024.02.05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4065,6 +4061,18 @@
   </si>
   <si>
     <t>D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SL-640</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uncooled Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rev.2024.02.20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4576,7 +4584,7 @@
   <dimension ref="B1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4590,8 +4598,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
+      <c r="M1" t="s">
+        <v>430</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>431</v>
+      </c>
       <c r="O1" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="2:15" s="2" customFormat="1">
@@ -5757,7 +5771,7 @@
         <v>401</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="O26" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5803,7 +5817,7 @@
         <v>402</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="O27" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5849,7 +5863,7 @@
         <v>403</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="O28" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5895,7 +5909,7 @@
         <v>404</v>
       </c>
       <c r="N29" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="O29" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5941,7 +5955,7 @@
         <v>416</v>
       </c>
       <c r="N30" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="O30" s="3" t="str">
         <f t="shared" si="3"/>
@@ -5953,7 +5967,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="M1:M1048576" numberStoredAsText="1"/>
+    <ignoredError sqref="M2:M1048576" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>